<commit_message>
merke skillerader mellom grupper
</commit_message>
<xml_diff>
--- a/src/main/resources/substituttlister/V2_stoler_med_oppreisingsfunksjon.xlsx
+++ b/src/main/resources/substituttlister/V2_stoler_med_oppreisingsfunksjon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aasmund/dev/hm-grunndata-alternativprodukter/src/main/resources/substituttlister/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{141E935B-E4F9-AD43-AE31-5FE8D15A6ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E681A5-CC35-C743-BA0A-D75D3534C16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3000" yWindow="-23760" windowWidth="26200" windowHeight="22740" firstSheet="1" activeTab="1" xr2:uid="{DAB7D3D8-04D0-4DD5-9B74-78B882D95CED}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="303">
   <si>
     <t>Delkontrakt</t>
   </si>
@@ -965,6 +965,9 @@
   </si>
   <si>
     <t>123458</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -2073,10 +2076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3485A8-7267-48FD-BE99-693AE922852B}">
-  <dimension ref="A1:E233"/>
+  <dimension ref="A1:E232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:XFD45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A239" sqref="A239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2146,6 +2149,9 @@
       <c r="E5" s="26"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="22"/>
@@ -2202,6 +2208,9 @@
       <c r="E11" s="26"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="22"/>
@@ -2238,12 +2247,15 @@
       <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="22"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="26" t="s">
         <v>14</v>
@@ -2253,7 +2265,7 @@
       </c>
       <c r="E17" s="26"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1"/>
       <c r="C18" s="26" t="s">
         <v>15</v>
@@ -2263,7 +2275,7 @@
       </c>
       <c r="E18" s="26"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="C19" s="26" t="s">
         <v>15</v>
@@ -2273,13 +2285,16 @@
       </c>
       <c r="E19" s="26"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="22"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="26" t="s">
         <v>16</v>
@@ -2289,7 +2304,7 @@
       </c>
       <c r="E21" s="26"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
       <c r="C22" s="26" t="s">
         <v>17</v>
@@ -2299,7 +2314,7 @@
       </c>
       <c r="E22" s="26"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="26" t="s">
         <v>17</v>
@@ -2309,7 +2324,7 @@
       </c>
       <c r="E23" s="26"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
       <c r="C24" s="26" t="s">
         <v>18</v>
@@ -2319,7 +2334,7 @@
       </c>
       <c r="E24" s="26"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
       <c r="C25" s="26" t="s">
         <v>18</v>
@@ -2329,13 +2344,16 @@
       </c>
       <c r="E25" s="26"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="22"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" s="1"/>
       <c r="C27" s="26" t="s">
         <v>19</v>
@@ -2345,7 +2363,7 @@
       </c>
       <c r="E27" s="26"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="1"/>
       <c r="C28" s="26" t="s">
         <v>20</v>
@@ -2355,7 +2373,7 @@
       </c>
       <c r="E28" s="28"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1"/>
       <c r="C29" s="26" t="s">
         <v>20</v>
@@ -2365,7 +2383,7 @@
       </c>
       <c r="E29" s="26"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
       <c r="C30" s="26" t="s">
         <v>21</v>
@@ -2375,7 +2393,7 @@
       </c>
       <c r="E30" s="26"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" s="1"/>
       <c r="C31" s="26" t="s">
         <v>21</v>
@@ -2385,13 +2403,16 @@
       </c>
       <c r="E31" s="26"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="22"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1"/>
       <c r="C33" s="26" t="s">
         <v>22</v>
@@ -2401,7 +2422,7 @@
       </c>
       <c r="E33" s="26"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" s="1"/>
       <c r="C34" s="26" t="s">
         <v>23</v>
@@ -2411,7 +2432,7 @@
       </c>
       <c r="E34" s="26"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
       <c r="C35" s="26" t="s">
         <v>23</v>
@@ -2421,7 +2442,7 @@
       </c>
       <c r="E35" s="26"/>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
       <c r="C36" s="26" t="s">
         <v>24</v>
@@ -2431,13 +2452,16 @@
       </c>
       <c r="E36" s="26"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="22"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" s="1"/>
       <c r="C38" s="26" t="s">
         <v>26</v>
@@ -2447,7 +2471,7 @@
       </c>
       <c r="E38" s="26"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1"/>
       <c r="C39" s="26" t="s">
         <v>27</v>
@@ -2457,7 +2481,7 @@
       </c>
       <c r="E39" s="26"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B40" s="1"/>
       <c r="C40" s="26" t="s">
         <v>27</v>
@@ -2467,7 +2491,7 @@
       </c>
       <c r="E40" s="26"/>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" s="1"/>
       <c r="C41" s="26" t="s">
         <v>28</v>
@@ -2477,13 +2501,16 @@
       </c>
       <c r="E41" s="26"/>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B42" s="1"/>
       <c r="C42" s="26"/>
       <c r="D42" s="27"/>
       <c r="E42" s="26"/>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
       <c r="C43" s="26" t="s">
         <v>29</v>
@@ -2493,7 +2520,7 @@
       </c>
       <c r="E43" s="26"/>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" s="1"/>
       <c r="C44" s="26" t="s">
         <v>30</v>
@@ -2503,13 +2530,16 @@
       </c>
       <c r="E44" s="26"/>
     </row>
-    <row r="45" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="B45" s="1"/>
       <c r="C45" s="26"/>
       <c r="D45" s="27"/>
       <c r="E45" s="26"/>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B46" s="1"/>
       <c r="C46" s="2" t="s">
         <v>31</v>
@@ -2518,7 +2548,7 @@
         <v>296140</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
         <v>32</v>
       </c>
@@ -2526,7 +2556,7 @@
         <v>240534</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
         <v>33</v>
       </c>
@@ -2534,7 +2564,12 @@
         <v>195627</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1"/>
       <c r="C50" s="2" t="s">
         <v>34</v>
@@ -2543,7 +2578,7 @@
         <v>296141</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
         <v>35</v>
       </c>
@@ -2551,7 +2586,7 @@
         <v>240533</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
         <v>36</v>
       </c>
@@ -2559,7 +2594,12 @@
         <v>195626</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
         <v>37</v>
@@ -2568,7 +2608,7 @@
         <v>296142</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
         <v>38</v>
       </c>
@@ -2576,7 +2616,7 @@
         <v>296310</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
         <v>39</v>
       </c>
@@ -2584,7 +2624,7 @@
         <v>296312</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
         <v>40</v>
       </c>
@@ -2592,7 +2632,7 @@
         <v>295771</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
         <v>41</v>
       </c>
@@ -2600,7 +2640,7 @@
         <v>295772</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C59" s="2" t="s">
         <v>42</v>
       </c>
@@ -2608,7 +2648,7 @@
         <v>240536</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C60" s="2" t="s">
         <v>43</v>
       </c>
@@ -2616,7 +2656,7 @@
         <v>195735</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C61" s="2" t="s">
         <v>44</v>
       </c>
@@ -2624,7 +2664,12 @@
         <v>195733</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
       <c r="C63" s="2" t="s">
         <v>45</v>
@@ -2633,7 +2678,7 @@
         <v>296143</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C64" s="2" t="s">
         <v>46</v>
       </c>
@@ -2641,7 +2686,7 @@
         <v>296311</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C65" s="2" t="s">
         <v>47</v>
       </c>
@@ -2649,7 +2694,7 @@
         <v>296313</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C66" s="2" t="s">
         <v>48</v>
       </c>
@@ -2657,7 +2702,7 @@
         <v>295766</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C67" s="2" t="s">
         <v>49</v>
       </c>
@@ -2665,7 +2710,7 @@
         <v>295767</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C68" s="2" t="s">
         <v>50</v>
       </c>
@@ -2673,7 +2718,7 @@
         <v>240535</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C69" s="2" t="s">
         <v>51</v>
       </c>
@@ -2681,7 +2726,7 @@
         <v>195734</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C70" s="2" t="s">
         <v>52</v>
       </c>
@@ -2689,7 +2734,12 @@
         <v>195732</v>
       </c>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C72" s="2" t="s">
         <v>53</v>
       </c>
@@ -2697,7 +2747,7 @@
         <v>296144</v>
       </c>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C73" s="2" t="s">
         <v>38</v>
       </c>
@@ -2705,7 +2755,7 @@
         <v>296310</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C74" s="2" t="s">
         <v>54</v>
       </c>
@@ -2713,7 +2763,7 @@
         <v>296312</v>
       </c>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C75" s="2" t="s">
         <v>55</v>
       </c>
@@ -2721,7 +2771,7 @@
         <v>295773</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C76" s="2" t="s">
         <v>56</v>
       </c>
@@ -2729,7 +2779,7 @@
         <v>295774</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C77" s="2" t="s">
         <v>57</v>
       </c>
@@ -2737,7 +2787,7 @@
         <v>240538</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C78" s="2" t="s">
         <v>58</v>
       </c>
@@ -2745,7 +2795,7 @@
         <v>195625</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C79" s="2" t="s">
         <v>59</v>
       </c>
@@ -2753,7 +2803,7 @@
         <v>195633</v>
       </c>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C80" s="2" t="s">
         <v>60</v>
       </c>
@@ -2761,7 +2811,7 @@
         <v>195739</v>
       </c>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C81" s="2" t="s">
         <v>61</v>
       </c>
@@ -2769,7 +2819,12 @@
         <v>195737</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C83" s="2" t="s">
         <v>62</v>
       </c>
@@ -2777,7 +2832,7 @@
         <v>296145</v>
       </c>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C84" s="2" t="s">
         <v>63</v>
       </c>
@@ -2785,7 +2840,7 @@
         <v>296311</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C85" s="2" t="s">
         <v>64</v>
       </c>
@@ -2793,7 +2848,7 @@
         <v>296313</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C86" s="2" t="s">
         <v>65</v>
       </c>
@@ -2801,7 +2856,7 @@
         <v>295768</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C87" s="2" t="s">
         <v>66</v>
       </c>
@@ -2809,7 +2864,7 @@
         <v>295769</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C88" s="2" t="s">
         <v>67</v>
       </c>
@@ -2817,7 +2872,7 @@
         <v>240537</v>
       </c>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C89" s="2" t="s">
         <v>68</v>
       </c>
@@ -2825,7 +2880,7 @@
         <v>195624</v>
       </c>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C90" s="2" t="s">
         <v>69</v>
       </c>
@@ -2833,7 +2888,7 @@
         <v>195632</v>
       </c>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C91" s="2" t="s">
         <v>70</v>
       </c>
@@ -2841,7 +2896,7 @@
         <v>195738</v>
       </c>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C92" s="2" t="s">
         <v>71</v>
       </c>
@@ -2849,7 +2904,12 @@
         <v>195736</v>
       </c>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
         <v>72</v>
       </c>
@@ -2857,7 +2917,7 @@
         <v>296146</v>
       </c>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
         <v>73</v>
       </c>
@@ -2865,7 +2925,7 @@
         <v>296306</v>
       </c>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
         <v>74</v>
       </c>
@@ -2873,7 +2933,7 @@
         <v>296308</v>
       </c>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
         <v>75</v>
       </c>
@@ -2881,7 +2941,7 @@
         <v>296314</v>
       </c>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C98" s="2" t="s">
         <v>76</v>
       </c>
@@ -2889,7 +2949,7 @@
         <v>295775</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C99" s="2" t="s">
         <v>77</v>
       </c>
@@ -2897,7 +2957,7 @@
         <v>240540</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C100" s="2" t="s">
         <v>58</v>
       </c>
@@ -2905,7 +2965,7 @@
         <v>195625</v>
       </c>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C101" s="2" t="s">
         <v>59</v>
       </c>
@@ -2913,7 +2973,7 @@
         <v>195633</v>
       </c>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C102" s="2" t="s">
         <v>78</v>
       </c>
@@ -2921,10 +2981,13 @@
         <v>195741</v>
       </c>
     </row>
-    <row r="103" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="D103" s="21"/>
     </row>
-    <row r="104" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C104" s="2" t="s">
         <v>79</v>
       </c>
@@ -2932,7 +2995,7 @@
         <v>296147</v>
       </c>
     </row>
-    <row r="105" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C105" s="2" t="s">
         <v>80</v>
       </c>
@@ -2940,7 +3003,7 @@
         <v>296307</v>
       </c>
     </row>
-    <row r="106" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C106" s="2" t="s">
         <v>81</v>
       </c>
@@ -2948,7 +3011,7 @@
         <v>296309</v>
       </c>
     </row>
-    <row r="107" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C107" s="2" t="s">
         <v>82</v>
       </c>
@@ -2956,7 +3019,7 @@
         <v>296315</v>
       </c>
     </row>
-    <row r="108" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C108" s="2" t="s">
         <v>83</v>
       </c>
@@ -2964,7 +3027,7 @@
         <v>295770</v>
       </c>
     </row>
-    <row r="109" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C109" s="2" t="s">
         <v>84</v>
       </c>
@@ -2972,7 +3035,7 @@
         <v>240539</v>
       </c>
     </row>
-    <row r="110" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C110" s="2" t="s">
         <v>68</v>
       </c>
@@ -2980,7 +3043,7 @@
         <v>195624</v>
       </c>
     </row>
-    <row r="111" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C111" s="2" t="s">
         <v>85</v>
       </c>
@@ -2988,10 +3051,13 @@
         <v>195740</v>
       </c>
     </row>
-    <row r="112" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="D112" s="21"/>
     </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C113" s="2" t="s">
         <v>86</v>
       </c>
@@ -2999,7 +3065,7 @@
         <v>296148</v>
       </c>
     </row>
-    <row r="114" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C114" s="2" t="s">
         <v>87</v>
       </c>
@@ -3007,7 +3073,7 @@
         <v>295777</v>
       </c>
     </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C115" s="2" t="s">
         <v>88</v>
       </c>
@@ -3015,7 +3081,7 @@
         <v>240522</v>
       </c>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C116" s="2" t="s">
         <v>89</v>
       </c>
@@ -3023,7 +3089,7 @@
         <v>195743</v>
       </c>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C117" s="2" t="s">
         <v>90</v>
       </c>
@@ -3031,7 +3097,12 @@
         <v>195637</v>
       </c>
     </row>
-    <row r="119" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C119" s="2" t="s">
         <v>91</v>
       </c>
@@ -3039,7 +3110,7 @@
         <v>296149</v>
       </c>
     </row>
-    <row r="120" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C120" s="2" t="s">
         <v>92</v>
       </c>
@@ -3047,7 +3118,7 @@
         <v>295776</v>
       </c>
     </row>
-    <row r="121" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C121" s="2" t="s">
         <v>93</v>
       </c>
@@ -3055,7 +3126,7 @@
         <v>240521</v>
       </c>
     </row>
-    <row r="122" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C122" s="2" t="s">
         <v>94</v>
       </c>
@@ -3063,7 +3134,7 @@
         <v>195742</v>
       </c>
     </row>
-    <row r="123" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C123" s="2" t="s">
         <v>95</v>
       </c>
@@ -3071,7 +3142,12 @@
         <v>195636</v>
       </c>
     </row>
-    <row r="125" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C125" s="2" t="s">
         <v>96</v>
       </c>
@@ -3079,7 +3155,7 @@
         <v>296316</v>
       </c>
     </row>
-    <row r="126" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C126" s="2" t="s">
         <v>97</v>
       </c>
@@ -3087,7 +3163,7 @@
         <v>296318</v>
       </c>
     </row>
-    <row r="127" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C127" s="2" t="s">
         <v>98</v>
       </c>
@@ -3095,7 +3171,7 @@
         <v>296324</v>
       </c>
     </row>
-    <row r="128" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C128" s="2" t="s">
         <v>99</v>
       </c>
@@ -3103,7 +3179,7 @@
         <v>241480</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C129" s="2" t="s">
         <v>100</v>
       </c>
@@ -3111,7 +3187,7 @@
         <v>241475</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C130" s="2" t="s">
         <v>101</v>
       </c>
@@ -3119,7 +3195,7 @@
         <v>241460</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C131" s="2" t="s">
         <v>100</v>
       </c>
@@ -3127,7 +3203,7 @@
         <v>241476</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C132" s="2" t="s">
         <v>102</v>
       </c>
@@ -3135,7 +3211,7 @@
         <v>241478</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C133" s="2" t="s">
         <v>103</v>
       </c>
@@ -3143,7 +3219,7 @@
         <v>241456</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C134" s="2" t="s">
         <v>104</v>
       </c>
@@ -3151,7 +3227,7 @@
         <v>241458</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C135" s="2" t="s">
         <v>105</v>
       </c>
@@ -3159,7 +3235,7 @@
         <v>296164</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C136" s="2" t="s">
         <v>106</v>
       </c>
@@ -3167,7 +3243,7 @@
         <v>240550</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C137" s="2" t="s">
         <v>107</v>
       </c>
@@ -3175,7 +3251,7 @@
         <v>240530</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C138" s="2" t="s">
         <v>108</v>
       </c>
@@ -3183,7 +3259,7 @@
         <v>195742</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C139" s="2" t="s">
         <v>109</v>
       </c>
@@ -3191,7 +3267,12 @@
         <v>195752</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B141" s="1"/>
       <c r="C141" s="2" t="s">
         <v>110</v>
@@ -3200,7 +3281,7 @@
         <v>296162</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C142" s="2" t="s">
         <v>111</v>
       </c>
@@ -3208,7 +3289,7 @@
         <v>240548</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C143" s="2" t="s">
         <v>112</v>
       </c>
@@ -3216,7 +3297,7 @@
         <v>240528</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C144" s="2" t="s">
         <v>113</v>
       </c>
@@ -3224,7 +3305,7 @@
         <v>195744</v>
       </c>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C145" s="2" t="s">
         <v>114</v>
       </c>
@@ -3232,7 +3313,7 @@
         <v>195750</v>
       </c>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C146" s="2" t="s">
         <v>115</v>
       </c>
@@ -3240,7 +3321,7 @@
         <v>195760</v>
       </c>
     </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C147" s="2" t="s">
         <v>116</v>
       </c>
@@ -3248,7 +3329,7 @@
         <v>296320</v>
       </c>
     </row>
-    <row r="148" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C148" s="2" t="s">
         <v>117</v>
       </c>
@@ -3256,7 +3337,7 @@
         <v>296322</v>
       </c>
     </row>
-    <row r="149" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C149" s="2" t="s">
         <v>118</v>
       </c>
@@ -3264,7 +3345,7 @@
         <v>241484</v>
       </c>
     </row>
-    <row r="150" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C150" s="2" t="s">
         <v>119</v>
       </c>
@@ -3272,7 +3353,7 @@
         <v>241482</v>
       </c>
     </row>
-    <row r="151" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C151" s="2" t="s">
         <v>120</v>
       </c>
@@ -3280,7 +3361,7 @@
         <v>241464</v>
       </c>
     </row>
-    <row r="152" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C152" s="2" t="s">
         <v>121</v>
       </c>
@@ -3288,7 +3369,12 @@
         <v>241462</v>
       </c>
     </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C154" s="2" t="s">
         <v>122</v>
       </c>
@@ -3296,7 +3382,7 @@
         <v>240544</v>
       </c>
     </row>
-    <row r="155" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C155" s="2" t="s">
         <v>123</v>
       </c>
@@ -3304,566 +3390,615 @@
         <v>240524</v>
       </c>
     </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B158" s="1"/>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B157" s="1"/>
+      <c r="C157" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D157" s="21">
+        <v>296160</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C158" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D158" s="21">
-        <v>296160</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4" x14ac:dyDescent="0.2">
+        <v>240546</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C159" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D159" s="21">
-        <v>240546</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.2">
+        <v>195746</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C160" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D160" s="21">
-        <v>195746</v>
-      </c>
-    </row>
-    <row r="161" spans="3:4" x14ac:dyDescent="0.2">
+        <v>195748</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C161" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D161" s="21">
-        <v>195748</v>
-      </c>
-    </row>
-    <row r="162" spans="3:4" x14ac:dyDescent="0.2">
+        <v>195756</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C162" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D162" s="21">
+        <v>195758</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C163" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D162" s="21">
-        <v>195756</v>
-      </c>
-    </row>
-    <row r="163" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C163" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="D163" s="21">
-        <v>195758</v>
-      </c>
-    </row>
-    <row r="164" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C164" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D164" s="21">
         <v>195757</v>
       </c>
     </row>
-    <row r="166" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C165" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D165" s="21">
+        <v>296317</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C166" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D166" s="21">
-        <v>296317</v>
-      </c>
-    </row>
-    <row r="167" spans="3:4" x14ac:dyDescent="0.2">
+        <v>296319</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C167" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D167" s="21">
-        <v>296319</v>
-      </c>
-    </row>
-    <row r="168" spans="3:4" x14ac:dyDescent="0.2">
+        <v>296325</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C168" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D168" s="21">
-        <v>296325</v>
-      </c>
-    </row>
-    <row r="169" spans="3:4" x14ac:dyDescent="0.2">
+        <v>296165</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C169" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D169" s="21">
-        <v>296165</v>
-      </c>
-    </row>
-    <row r="170" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241479</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C170" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D170" s="21">
-        <v>241479</v>
-      </c>
-    </row>
-    <row r="171" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241477</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C171" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D171" s="21">
-        <v>241477</v>
-      </c>
-    </row>
-    <row r="172" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241459</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C172" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D172" s="21">
-        <v>241459</v>
-      </c>
-    </row>
-    <row r="173" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241455</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C173" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D173" s="21">
-        <v>241455</v>
-      </c>
-    </row>
-    <row r="174" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241457</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C174" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D174" s="21">
-        <v>241457</v>
-      </c>
-    </row>
-    <row r="175" spans="3:4" x14ac:dyDescent="0.2">
+        <v>240549</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C175" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D175" s="21">
-        <v>240549</v>
-      </c>
-    </row>
-    <row r="176" spans="3:4" x14ac:dyDescent="0.2">
+        <v>240529</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C176" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D176" s="21">
-        <v>240529</v>
-      </c>
-    </row>
-    <row r="177" spans="3:4" x14ac:dyDescent="0.2">
+        <v>195743</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C177" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D177" s="21">
-        <v>195743</v>
-      </c>
-    </row>
-    <row r="178" spans="3:4" x14ac:dyDescent="0.2">
+        <v>195753</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C178" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D178" s="21">
-        <v>195753</v>
-      </c>
-    </row>
-    <row r="179" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C179" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D179" s="21">
         <v>195761</v>
       </c>
     </row>
-    <row r="181" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C180" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D180" s="21">
+        <v>296321</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C181" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D181" s="21">
-        <v>296321</v>
-      </c>
-    </row>
-    <row r="182" spans="3:4" x14ac:dyDescent="0.2">
+        <v>296323</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C182" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D182" s="21">
-        <v>296323</v>
-      </c>
-    </row>
-    <row r="183" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241483</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C183" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D183" s="21">
-        <v>241483</v>
-      </c>
-    </row>
-    <row r="184" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241481</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C184" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D184" s="21">
-        <v>241481</v>
-      </c>
-    </row>
-    <row r="185" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241463</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C185" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D185" s="21">
-        <v>241463</v>
-      </c>
-    </row>
-    <row r="186" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241461</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C186" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D186" s="21">
-        <v>241461</v>
-      </c>
-    </row>
-    <row r="187" spans="3:4" x14ac:dyDescent="0.2">
+        <v>296163</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C187" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D187" s="21">
-        <v>296163</v>
-      </c>
-    </row>
-    <row r="188" spans="3:4" x14ac:dyDescent="0.2">
+        <v>240547</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C188" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D188" s="21">
-        <v>240547</v>
-      </c>
-    </row>
-    <row r="189" spans="3:4" x14ac:dyDescent="0.2">
+        <v>240527</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C189" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D189" s="21">
-        <v>240527</v>
-      </c>
-    </row>
-    <row r="190" spans="3:4" x14ac:dyDescent="0.2">
+        <v>195745</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C190" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D190" s="21">
-        <v>195745</v>
-      </c>
-    </row>
-    <row r="191" spans="3:4" x14ac:dyDescent="0.2">
+        <v>195755</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C191" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D191" s="21">
-        <v>195755</v>
-      </c>
-    </row>
-    <row r="192" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C192" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D192" s="21">
         <v>195751</v>
       </c>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="D193" s="21"/>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B194" s="1"/>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D192" s="21"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B193" s="1"/>
+      <c r="C193" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D193" s="21">
+        <v>296159</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C194" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D194" s="21">
-        <v>296159</v>
-      </c>
-    </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
+        <v>240523</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C195" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D195" s="21">
-        <v>240523</v>
-      </c>
-    </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C196" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D196" s="21">
         <v>240543</v>
       </c>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B198" s="1"/>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B197" s="1"/>
+      <c r="C197" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D197" s="21">
+        <v>296161</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C198" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D198" s="21">
-        <v>296161</v>
-      </c>
-    </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
+        <v>195747</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C199" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D199" s="21">
-        <v>195747</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
+        <v>195749</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C200" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D200" s="21">
-        <v>195749</v>
-      </c>
-    </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C201" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D201" s="21">
         <v>195759</v>
       </c>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C202" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D202" s="21">
+        <v>296166</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C203" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D203" s="21">
-        <v>296166</v>
-      </c>
-    </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
+        <v>295789</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C204" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D204" s="21">
-        <v>295789</v>
-      </c>
-    </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
+        <v>240552</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C205" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D205" s="21">
-        <v>240552</v>
-      </c>
-    </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
+        <v>241081</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C206" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D206" s="21">
-        <v>241081</v>
-      </c>
-    </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
+        <v>196200</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C207" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D207" s="21">
-        <v>196200</v>
-      </c>
-    </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C208" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D208" s="21">
         <v>195762</v>
       </c>
     </row>
-    <row r="210" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C209" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D209" s="21">
+        <v>296167</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C210" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D210" s="21">
-        <v>296167</v>
-      </c>
-    </row>
-    <row r="211" spans="3:4" x14ac:dyDescent="0.2">
+        <v>295788</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C211" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D211" s="21">
-        <v>295788</v>
-      </c>
-    </row>
-    <row r="212" spans="3:4" x14ac:dyDescent="0.2">
+        <v>240551</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C212" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D212" s="21">
-        <v>240551</v>
-      </c>
-    </row>
-    <row r="213" spans="3:4" x14ac:dyDescent="0.2">
+        <v>241080</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C213" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D213" s="21">
-        <v>241080</v>
-      </c>
-    </row>
-    <row r="214" spans="3:4" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="D213" s="25">
+        <v>196199</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C214" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D214" s="25">
-        <v>196199</v>
-      </c>
-    </row>
-    <row r="215" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C215" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D215" s="24">
+      <c r="D214" s="24">
         <v>195763</v>
       </c>
     </row>
-    <row r="216" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D216" s="24"/>
-    </row>
-    <row r="217" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D215" s="24"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C216" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D216" s="21">
+        <v>196820</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C217" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D217" s="21">
-        <v>196820</v>
-      </c>
-    </row>
-    <row r="218" spans="3:4" x14ac:dyDescent="0.2">
+        <v>251670</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C218" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D218" s="21">
-        <v>251670</v>
-      </c>
-    </row>
-    <row r="219" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C219" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D219" s="21">
         <v>215297</v>
       </c>
     </row>
-    <row r="221" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C220" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D220" s="21">
+        <v>248794</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C221" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D221" s="21">
-        <v>248794</v>
-      </c>
-    </row>
-    <row r="222" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C222" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D222" s="21">
         <v>269870</v>
       </c>
     </row>
-    <row r="223" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D223" s="21"/>
-    </row>
-    <row r="224" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C224" s="29" t="s">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D222" s="21"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C223" s="29" t="s">
         <v>180</v>
       </c>
+      <c r="D223" s="27">
+        <v>296288</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C224" s="26" t="s">
+        <v>181</v>
+      </c>
       <c r="D224" s="27">
-        <v>296288</v>
-      </c>
-    </row>
-    <row r="225" spans="3:5" x14ac:dyDescent="0.2">
+        <v>296289</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C225" s="26" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D225" s="27">
-        <v>296289</v>
-      </c>
-    </row>
-    <row r="226" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C226" s="26" t="s">
-        <v>182</v>
-      </c>
-      <c r="D226" s="27">
         <v>296290</v>
       </c>
     </row>
-    <row r="228" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A226" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C227" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D227" s="27">
+        <v>296285</v>
+      </c>
+      <c r="E227" s="28"/>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C228" s="26" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D228" s="27">
-        <v>296285</v>
-      </c>
-      <c r="E228" s="28"/>
-    </row>
-    <row r="229" spans="3:5" x14ac:dyDescent="0.2">
+        <v>244819</v>
+      </c>
+      <c r="E228" s="26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C229" s="26" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D229" s="27">
-        <v>244819</v>
-      </c>
-      <c r="E229" s="26" t="s">
+        <v>296286</v>
+      </c>
+      <c r="E229" s="28"/>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C230" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="D230" s="27">
+        <v>239900</v>
+      </c>
+      <c r="E230" s="26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C230" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="D230" s="27">
-        <v>296286</v>
-      </c>
-      <c r="E230" s="28"/>
-    </row>
-    <row r="231" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C231" s="26" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D231" s="27">
-        <v>239900</v>
-      </c>
-      <c r="E231" s="26" t="s">
+        <v>296287</v>
+      </c>
+      <c r="E231" s="28"/>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C232" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D232" s="27">
+        <v>236421</v>
+      </c>
+      <c r="E232" s="26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="232" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C232" s="26" t="s">
-        <v>187</v>
-      </c>
-      <c r="D232" s="27">
-        <v>296287</v>
-      </c>
-      <c r="E232" s="28"/>
-    </row>
-    <row r="233" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C233" s="26" t="s">
-        <v>188</v>
-      </c>
-      <c r="D233" s="27">
-        <v>236421</v>
-      </c>
-      <c r="E233" s="26" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D214">
+  <conditionalFormatting sqref="D213">
     <cfRule type="duplicateValues" dxfId="6" priority="1" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="5" priority="2" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="4" priority="3" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="3" priority="4" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D215:D216">
+  <conditionalFormatting sqref="D214:D215">
     <cfRule type="duplicateValues" dxfId="2" priority="8" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="1" priority="9" stopIfTrue="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="10" stopIfTrue="1"/>

</xml_diff>